<commit_message>
data : case 1
</commit_message>
<xml_diff>
--- a/data/case1/1/details_14.xlsx
+++ b/data/case1/1/details_14.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9262" windowHeight="4935"/>
+    <workbookView windowWidth="12225" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -386,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -492,156 +492,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -698,34 +700,34 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
       <border>
@@ -736,7 +738,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -764,36 +766,36 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </horizontal>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
       <border>
         <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
       <border>
         <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </bottom>
       </border>
     </dxf>
@@ -808,19 +810,19 @@
       </font>
       <border>
         <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
       <border>
@@ -835,59 +837,59 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
       <border>
         <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </top>
         <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b val="true"/>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79998168889431"/>
+          <bgColor theme="4" tint="0.79998168889431"/>
         </patternFill>
       </fill>
       <border>
         <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39997558519242"/>
         </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="false" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -896,7 +898,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+    <tableStyle name="PivotStylePreset2_Accent1" table="false" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1177,74 +1179,82 @@
   <sheetPr/>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L3"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="2.14159292035398" customWidth="1"/>
-    <col min="3" max="3" width="2.5929203539823" customWidth="1"/>
-    <col min="4" max="4" width="3.14159292035398" customWidth="1"/>
-    <col min="5" max="5" width="2.14159292035398" customWidth="1"/>
-    <col min="6" max="7" width="3.14159292035398" customWidth="1"/>
-    <col min="8" max="8" width="2.14159292035398" customWidth="1"/>
-    <col min="9" max="12" width="3.14159292035398" customWidth="1"/>
-    <col min="13" max="16" width="5.70796460176991" customWidth="1"/>
-    <col min="17" max="17" width="4.70796460176991" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="true"/>
+    <col min="3" max="3" width="2.140625" customWidth="true"/>
+    <col min="5" max="5" width="2.140625" customWidth="true"/>
+    <col min="6" max="6" width="3.140625" customWidth="true"/>
+    <col min="13" max="13" width="5.7109375" customWidth="true"/>
+    <col min="17" max="17" width="4.7109375" customWidth="true"/>
+    <col min="2" max="2" width="2.140625" customWidth="true"/>
+    <col min="4" max="4" width="3.140625" customWidth="true"/>
+    <col min="7" max="7" width="3.140625" customWidth="true"/>
+    <col min="8" max="8" width="2.140625" customWidth="true"/>
+    <col min="9" max="9" width="3.140625" customWidth="true"/>
+    <col min="10" max="10" width="3.140625" customWidth="true"/>
+    <col min="11" max="11" width="3.140625" customWidth="true"/>
+    <col min="12" max="12" width="3.140625" customWidth="true"/>
+    <col min="14" max="14" width="5.7109375" customWidth="true"/>
+    <col min="15" max="15" width="5.7109375" customWidth="true"/>
+    <col min="16" max="16" width="5.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1">
+    <row r="1">
+      <c r="A1" s="0">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="0">
         <v>5</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="0">
+        <v>7</v>
+      </c>
+      <c r="D1" s="0">
         <v>11</v>
       </c>
-      <c r="D1">
-        <v>7</v>
-      </c>
-      <c r="E1">
+      <c r="E1" s="0">
         <v>9</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="0">
         <v>29</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="0">
         <v>21</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="0">
         <v>2</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="0">
+        <v>16</v>
+      </c>
+      <c r="J1" s="0">
+        <v>12</v>
+      </c>
+      <c r="K1" s="0">
+        <v>19</v>
+      </c>
+      <c r="L1" s="0">
         <v>17</v>
       </c>
-      <c r="J1">
-        <v>12</v>
-      </c>
-      <c r="K1">
-        <v>19</v>
-      </c>
-      <c r="L1">
-        <v>16</v>
-      </c>
-      <c r="M1">
-        <v>0.059</v>
-      </c>
-      <c r="N1">
-        <v>0.092</v>
-      </c>
-      <c r="O1">
-        <v>0.081</v>
-      </c>
-      <c r="P1">
-        <v>0.046</v>
-      </c>
-      <c r="Q1">
-        <v>0.06</v>
+      <c r="M1" s="0">
+        <v>0.058999999999999997</v>
+      </c>
+      <c r="N1" s="0">
+        <v>0.091999999999999998</v>
+      </c>
+      <c r="O1" s="0">
+        <v>0.081000000000000003</v>
+      </c>
+      <c r="P1" s="0">
+        <v>0.045999999999999999</v>
+      </c>
+      <c r="Q1" s="0">
+        <v>0.059999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>